<commit_message>
* Update DEMO-Data * Finalization altitude correction * Fv_veh calculation update (now option 2 is the new preferred one) Option 2 is deleted from result file
</commit_message>
<xml_diff>
--- a/Docs/GenericData.xlsx
+++ b/Docs/GenericData.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\TE-Em\Projekte\I_2013_08_HDV_CO2_LOT_4_SR7\VECTO-CSE\Functions\V3.0\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12585" yWindow="-15" windowWidth="12630" windowHeight="11205" tabRatio="759"/>
+    <workbookView xWindow="12585" yWindow="-15" windowWidth="12630" windowHeight="11205" tabRatio="759" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GenShape" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,7 @@
   <definedNames>
     <definedName name="RigidSolo">Input_ACEA!$S$9:$S$19</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -29,9 +34,6 @@
   </si>
   <si>
     <t>fape</t>
-  </si>
-  <si>
-    <t>c Description</t>
   </si>
   <si>
     <t>X</t>
@@ -151,22 +153,25 @@
     <t>delta CdxA</t>
   </si>
   <si>
-    <t>rigid solo</t>
+    <t># Description</t>
   </si>
   <si>
-    <t>rigid trailer</t>
+    <t>rigid (solo)</t>
   </si>
   <si>
-    <t>tractor semitrailer</t>
+    <t>rigid &amp; trailer</t>
   </si>
   <si>
-    <t>coach bus</t>
+    <t>tractor &amp; semitrailer</t>
+  </si>
+  <si>
+    <t>coach / bus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
@@ -1283,14 +1288,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-AT"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1310,6 +1318,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Input_ACEA!$S$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rigid (solo)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:xVal>
             <c:numRef>
               <c:f>Input_ACEA!$R$9:$R$19</c:f>
@@ -1395,10 +1414,26 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F91E-4AB2-9937-A93B302FF383}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Input_ACEA!$T$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rigid &amp; trailer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:xVal>
             <c:numRef>
               <c:f>Input_ACEA!$R$9:$R$19</c:f>
@@ -1484,10 +1519,26 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F91E-4AB2-9937-A93B302FF383}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Input_ACEA!$U$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>tractor &amp; semitrailer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:xVal>
             <c:numRef>
               <c:f>Input_ACEA!$R$9:$R$19</c:f>
@@ -1573,10 +1624,26 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F91E-4AB2-9937-A93B302FF383}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Input_ACEA!$V$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>coach / bus</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:xVal>
             <c:numRef>
               <c:f>Input_ACEA!$R$9:$R$19</c:f>
@@ -1662,6 +1729,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F91E-4AB2-9937-A93B302FF383}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1671,49 +1743,115 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="229230080"/>
-        <c:axId val="229231616"/>
+        <c:axId val="235890176"/>
+        <c:axId val="235891712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="229230080"/>
+        <c:axId val="235890176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="6"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>yaw angle (beta) [°]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="229231616"/>
+        <c:crossAx val="235891712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="229231616"/>
+        <c:axId val="235891712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>delta CdxA</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="229230080"/>
+        <c:crossAx val="235890176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.65698556430446198"/>
+          <c:y val="6.3247302420530754E-2"/>
+          <c:w val="0.32356999125109359"/>
+          <c:h val="0.8503572470107903"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1600"/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1764,16 +1902,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1796,9 +1934,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1836,9 +1974,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1873,7 +2011,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1908,7 +2046,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2084,11 +2222,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="AJ5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AW19" sqref="AW19"/>
+      <selection pane="bottomRight" sqref="A1:AU15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2332,150 +2470,150 @@
     </row>
     <row r="4" spans="1:53" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="C4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="28" t="s">
-        <v>5</v>
-      </c>
       <c r="D4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="28" t="s">
-        <v>5</v>
-      </c>
       <c r="F4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="28" t="s">
-        <v>5</v>
-      </c>
       <c r="H4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="28" t="s">
-        <v>5</v>
-      </c>
       <c r="J4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="28" t="s">
-        <v>5</v>
-      </c>
       <c r="L4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="28" t="s">
-        <v>5</v>
-      </c>
       <c r="N4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="28" t="s">
-        <v>5</v>
-      </c>
       <c r="P4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="28" t="s">
-        <v>5</v>
-      </c>
       <c r="R4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="S4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="S4" s="28" t="s">
-        <v>5</v>
-      </c>
       <c r="T4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="U4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="U4" s="28" t="s">
-        <v>5</v>
-      </c>
       <c r="V4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="W4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="W4" s="28" t="s">
-        <v>5</v>
-      </c>
       <c r="X4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="Y4" s="28" t="s">
-        <v>5</v>
-      </c>
       <c r="Z4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="AA4" s="28" t="s">
-        <v>5</v>
-      </c>
       <c r="AB4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="AC4" s="28" t="s">
-        <v>5</v>
-      </c>
       <c r="AD4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="AE4" s="28" t="s">
-        <v>5</v>
-      </c>
       <c r="AF4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="AG4" s="28" t="s">
-        <v>5</v>
-      </c>
       <c r="AH4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="AI4" s="28" t="s">
-        <v>5</v>
-      </c>
       <c r="AJ4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="AK4" s="28" t="s">
-        <v>5</v>
-      </c>
       <c r="AL4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="AM4" s="28" t="s">
-        <v>5</v>
-      </c>
       <c r="AN4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="AO4" s="28" t="s">
-        <v>5</v>
-      </c>
       <c r="AP4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="AQ4" s="28" t="s">
-        <v>5</v>
-      </c>
       <c r="AR4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="AS4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="AS4" s="28" t="s">
-        <v>5</v>
-      </c>
       <c r="AT4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU4" s="28" t="s">
         <v>4</v>
-      </c>
-      <c r="AU4" s="28" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="39">
         <v>0</v>
@@ -2647,7 +2785,7 @@
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="39">
         <v>1</v>
@@ -2819,7 +2957,7 @@
     </row>
     <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="39">
         <v>2</v>
@@ -2991,7 +3129,7 @@
     </row>
     <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="39">
         <v>3</v>
@@ -3163,7 +3301,7 @@
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="39">
         <v>4</v>
@@ -3335,7 +3473,7 @@
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="39">
         <v>5</v>
@@ -3507,7 +3645,7 @@
     </row>
     <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="39">
         <v>6</v>
@@ -3679,7 +3817,7 @@
     </row>
     <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="39">
         <v>7</v>
@@ -3851,7 +3989,7 @@
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="39">
         <v>8</v>
@@ -4023,7 +4161,7 @@
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" s="39">
         <v>9</v>
@@ -4195,7 +4333,7 @@
     </row>
     <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="39">
         <v>10</v>
@@ -4389,8 +4527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="R3:V33"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9:U19"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4411,7 +4549,7 @@
     </row>
     <row r="4" spans="18:22" x14ac:dyDescent="0.25">
       <c r="R4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S4" s="41">
         <v>1.3526E-2</v>
@@ -4428,7 +4566,7 @@
     </row>
     <row r="5" spans="18:22" x14ac:dyDescent="0.25">
       <c r="R5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S5" s="41">
         <v>1.7746000000000001E-2</v>
@@ -4445,7 +4583,7 @@
     </row>
     <row r="6" spans="18:22" x14ac:dyDescent="0.25">
       <c r="R6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S6" s="41">
         <v>-6.6600000000000003E-4</v>
@@ -4462,19 +4600,19 @@
     </row>
     <row r="8" spans="18:22" x14ac:dyDescent="0.25">
       <c r="R8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T8" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U8" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="V8" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="18:22" x14ac:dyDescent="0.25">
@@ -4773,7 +4911,7 @@
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="51"/>
       <c r="B1" s="53" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="54"/>
       <c r="D1" s="54"/>
@@ -4788,19 +4926,19 @@
     </row>
     <row r="3" spans="1:5" ht="44.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="30" t="s">
         <v>11</v>
-      </c>
-      <c r="E3" s="30" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4808,13 +4946,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>14</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>15</v>
       </c>
       <c r="E4" s="32">
         <v>0</v>
@@ -4825,13 +4963,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>17</v>
       </c>
       <c r="E5" s="33">
         <v>1</v>
@@ -4841,10 +4979,10 @@
       <c r="A6" s="44"/>
       <c r="B6" s="47"/>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="34">
         <v>2</v>
@@ -4854,10 +4992,10 @@
       <c r="A7" s="44"/>
       <c r="B7" s="47"/>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="34">
         <v>3</v>
@@ -4867,10 +5005,10 @@
       <c r="A8" s="44"/>
       <c r="B8" s="47"/>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="34">
         <v>4</v>
@@ -4880,10 +5018,10 @@
       <c r="A9" s="44"/>
       <c r="B9" s="48"/>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" s="34">
         <v>5</v>
@@ -4892,13 +5030,13 @@
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="44"/>
       <c r="B10" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="E10" s="34">
         <v>6</v>
@@ -4908,10 +5046,10 @@
       <c r="A11" s="44"/>
       <c r="B11" s="47"/>
       <c r="C11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="34">
         <v>7</v>
@@ -4921,10 +5059,10 @@
       <c r="A12" s="45"/>
       <c r="B12" s="50"/>
       <c r="C12" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="35">
         <v>8</v>
@@ -4935,13 +5073,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="E13" s="33">
         <v>9</v>
@@ -4951,10 +5089,10 @@
       <c r="A14" s="44"/>
       <c r="B14" s="48"/>
       <c r="C14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E14" s="34">
         <v>10</v>
@@ -4963,13 +5101,13 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="44"/>
       <c r="B15" s="49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" s="34">
         <v>11</v>
@@ -4979,10 +5117,10 @@
       <c r="A16" s="44"/>
       <c r="B16" s="48"/>
       <c r="C16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16" s="34">
         <v>12</v>
@@ -4991,13 +5129,13 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="44"/>
       <c r="B17" s="49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E17" s="34">
         <v>13</v>
@@ -5007,10 +5145,10 @@
       <c r="A18" s="45"/>
       <c r="B18" s="50"/>
       <c r="C18" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E18" s="35">
         <v>14</v>
@@ -5021,13 +5159,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" s="33">
         <v>15</v>
@@ -5036,13 +5174,13 @@
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="44"/>
       <c r="B20" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E20" s="34">
         <v>16</v>
@@ -5051,13 +5189,13 @@
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="45"/>
       <c r="B21" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E21" s="35">
         <v>17</v>
@@ -5137,15 +5275,15 @@
     </row>
     <row r="4" spans="1:2" ht="44.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="31">
         <v>21</v>
@@ -5153,7 +5291,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="31">
         <v>22</v>
@@ -5161,7 +5299,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="31">
         <v>23</v>

</xml_diff>

<commit_message>
* Deletion of unused variables (omega_wh; omega_wh_acc; omega_p_wh_acc; t_tire; p_tire; ...) * Include of new variables for validity criteria (t_amb; t_ground; tq_grd) * Deletion of [ss.ss] coordinate input * Update criteria values * Include of reference vehicle high in genshape file * Expansion of the job-File due to new results * Expand vehicle file with vVehMax value * Check of digits after decimal seperator for all coordinates and transmission ratios (gear + axle) * Update GUI due to new criteria values * Option 2 result values deleted * Output files adapted * Calculation of new Result values (delta_CdxA_height; v_avg_LS/HS; t_amb_LS1) * Update of Excel DemoData file
</commit_message>
<xml_diff>
--- a/Docs/GenericData.xlsx
+++ b/Docs/GenericData.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\TE-Em\Projekte\I_2013_08_HDV_CO2_LOT_4_SR7\VECTO-CSE\Functions\V3.0\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12585" yWindow="-15" windowWidth="12630" windowHeight="11205" tabRatio="759" activeTab="1"/>
+    <workbookView xWindow="12585" yWindow="-15" windowWidth="12630" windowHeight="11205" tabRatio="759"/>
   </bookViews>
   <sheets>
     <sheet name="GenShape" sheetId="1" r:id="rId1"/>
@@ -20,12 +15,12 @@
   <definedNames>
     <definedName name="RigidSolo">Input_ACEA!$S$9:$S$19</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="44">
   <si>
     <t>vehclass</t>
   </si>
@@ -167,11 +162,14 @@
   <si>
     <t>coach / bus</t>
   </si>
+  <si>
+    <t>Href</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
@@ -1201,9 +1199,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1211,6 +1206,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1296,9 +1294,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="de-AT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1414,7 +1412,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F91E-4AB2-9937-A93B302FF383}"/>
             </c:ext>
@@ -1519,7 +1517,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F91E-4AB2-9937-A93B302FF383}"/>
             </c:ext>
@@ -1624,7 +1622,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-F91E-4AB2-9937-A93B302FF383}"/>
             </c:ext>
@@ -1729,7 +1727,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-F91E-4AB2-9937-A93B302FF383}"/>
             </c:ext>
@@ -1743,11 +1741,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="235890176"/>
-        <c:axId val="235891712"/>
+        <c:axId val="47530368"/>
+        <c:axId val="47532288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="235890176"/>
+        <c:axId val="47530368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1778,12 +1776,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235891712"/>
+        <c:crossAx val="47532288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="235891712"/>
+        <c:axId val="47532288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.5"/>
@@ -1814,7 +1812,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235890176"/>
+        <c:crossAx val="47530368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1934,9 +1932,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1974,9 +1972,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2011,7 +2009,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2046,7 +2044,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2220,13 +2218,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA20"/>
+  <dimension ref="A1:BA21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="AJ5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" sqref="A1:AU15"/>
+      <selection pane="bottomRight" activeCell="AW35" sqref="AW35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2469,484 +2467,386 @@
       </c>
     </row>
     <row r="4" spans="1:53" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="40">
+        <v>3.6</v>
+      </c>
+      <c r="D4" s="40">
+        <v>3.6</v>
+      </c>
+      <c r="F4" s="40">
+        <v>3.75</v>
+      </c>
+      <c r="H4" s="40">
+        <v>3.9</v>
+      </c>
+      <c r="J4" s="40">
+        <v>4</v>
+      </c>
+      <c r="L4" s="40">
+        <v>4</v>
+      </c>
+      <c r="N4" s="40">
+        <v>4</v>
+      </c>
+      <c r="P4" s="40">
+        <v>4</v>
+      </c>
+      <c r="R4" s="40">
+        <v>4</v>
+      </c>
+      <c r="T4" s="40">
+        <v>4</v>
+      </c>
+      <c r="V4" s="40">
+        <v>4</v>
+      </c>
+      <c r="X4" s="40">
+        <v>4</v>
+      </c>
+      <c r="Z4" s="40">
+        <v>4</v>
+      </c>
+      <c r="AB4" s="40">
+        <v>4</v>
+      </c>
+      <c r="AD4" s="40">
+        <v>4</v>
+      </c>
+      <c r="AF4" s="40">
+        <v>4</v>
+      </c>
+      <c r="AH4" s="40">
+        <v>4</v>
+      </c>
+      <c r="AJ4" s="40">
+        <v>4</v>
+      </c>
+      <c r="AL4" s="40">
+        <v>4</v>
+      </c>
+      <c r="AN4" s="40">
+        <v>4</v>
+      </c>
+      <c r="AP4" s="40">
+        <v>4</v>
+      </c>
+      <c r="AR4" s="40">
+        <v>4</v>
+      </c>
+      <c r="AT4" s="40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:53" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="28" t="s">
+      <c r="C5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="28" t="s">
+      <c r="E5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="28" t="s">
+      <c r="G5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="28" t="s">
+      <c r="I5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="L4" s="28" t="s">
+      <c r="K5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="N4" s="28" t="s">
+      <c r="M5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="N5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="P4" s="28" t="s">
+      <c r="O5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="Q4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="R4" s="28" t="s">
+      <c r="Q5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="R5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="S4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="T4" s="28" t="s">
+      <c r="S5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="T5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="U4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="V4" s="28" t="s">
+      <c r="U5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="V5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="W4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="X4" s="28" t="s">
+      <c r="W5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="X5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="Y4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z4" s="28" t="s">
+      <c r="Y5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="AA4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB4" s="28" t="s">
+      <c r="AA5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="AC4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD4" s="28" t="s">
+      <c r="AC5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="AE4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF4" s="28" t="s">
+      <c r="AE5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="AG4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="AH4" s="28" t="s">
+      <c r="AG5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="AI4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ4" s="28" t="s">
+      <c r="AI5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="AK4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="AL4" s="28" t="s">
+      <c r="AK5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="AM4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="AN4" s="28" t="s">
+      <c r="AM5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="AO4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="AP4" s="28" t="s">
+      <c r="AO5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="AQ4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="AR4" s="28" t="s">
+      <c r="AQ5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="AR5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="AS4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="AT4" s="28" t="s">
+      <c r="AS5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="AU4" s="28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="39">
-        <v>0</v>
-      </c>
-      <c r="C5" s="40">
-        <f>Input_ACEA!S9</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="39">
-        <v>0</v>
-      </c>
-      <c r="E5" s="40">
-        <f>Input_ACEA!S9</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="39">
-        <v>0</v>
-      </c>
-      <c r="G5" s="40">
-        <f>Input_ACEA!S9</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="39">
-        <v>0</v>
-      </c>
-      <c r="I5" s="40">
-        <f>Input_ACEA!S9</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="39">
-        <v>0</v>
-      </c>
-      <c r="K5" s="40">
-        <f>Input_ACEA!S9</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="39">
-        <v>0</v>
-      </c>
-      <c r="M5" s="40">
-        <f>Input_ACEA!T9</f>
-        <v>0</v>
-      </c>
-      <c r="N5" s="39">
-        <v>0</v>
-      </c>
-      <c r="O5" s="40">
-        <f>Input_ACEA!U9</f>
-        <v>0</v>
-      </c>
-      <c r="P5" s="39">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="40">
-        <f>Input_ACEA!S9</f>
-        <v>0</v>
-      </c>
-      <c r="R5" s="39">
-        <v>0</v>
-      </c>
-      <c r="S5" s="40">
-        <f>Input_ACEA!S9</f>
-        <v>0</v>
-      </c>
-      <c r="T5" s="39">
-        <v>0</v>
-      </c>
-      <c r="U5" s="40">
-        <f>Input_ACEA!U9</f>
-        <v>0</v>
-      </c>
-      <c r="V5" s="39">
-        <v>0</v>
-      </c>
-      <c r="W5" s="40">
-        <f>Input_ACEA!S9</f>
-        <v>0</v>
-      </c>
-      <c r="X5" s="39">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="40">
-        <f>Input_ACEA!T9</f>
-        <v>0</v>
-      </c>
-      <c r="Z5" s="39">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="40">
-        <f>Input_ACEA!U9</f>
-        <v>0</v>
-      </c>
-      <c r="AB5" s="39">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="40">
-        <f>Input_ACEA!S9</f>
-        <v>0</v>
-      </c>
-      <c r="AD5" s="39">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="40">
-        <f>Input_ACEA!U9</f>
-        <v>0</v>
-      </c>
-      <c r="AF5" s="39">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="40">
-        <f>Input_ACEA!S9</f>
-        <v>0</v>
-      </c>
-      <c r="AH5" s="39">
-        <v>0</v>
-      </c>
-      <c r="AI5" s="40">
-        <f>Input_ACEA!U9</f>
-        <v>0</v>
-      </c>
-      <c r="AJ5" s="39">
-        <v>0</v>
-      </c>
-      <c r="AK5" s="40">
-        <f>Input_ACEA!S9</f>
-        <v>0</v>
-      </c>
-      <c r="AL5" s="39">
-        <v>0</v>
-      </c>
-      <c r="AM5" s="40">
-        <f>Input_ACEA!S9</f>
-        <v>0</v>
-      </c>
-      <c r="AN5" s="39">
-        <v>0</v>
-      </c>
-      <c r="AO5" s="40">
-        <f>Input_ACEA!S9</f>
-        <v>0</v>
-      </c>
-      <c r="AP5" s="39">
-        <v>0</v>
-      </c>
-      <c r="AQ5" s="40">
-        <f>Input_ACEA!$V9</f>
-        <v>0</v>
-      </c>
-      <c r="AR5" s="39">
-        <v>0</v>
-      </c>
-      <c r="AS5" s="40">
-        <f>Input_ACEA!$V9</f>
-        <v>0</v>
-      </c>
-      <c r="AT5" s="39">
-        <v>0</v>
-      </c>
-      <c r="AU5" s="40">
-        <f>Input_ACEA!$V9</f>
-        <v>0</v>
-      </c>
-      <c r="AV5" s="24"/>
-      <c r="AW5" s="24"/>
-      <c r="AX5" s="24"/>
-      <c r="AY5" s="24"/>
-      <c r="AZ5" s="24"/>
-      <c r="BA5" s="24"/>
+      <c r="AU5" s="28" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="40">
-        <f>Input_ACEA!S10</f>
-        <v>3.0606000000000001E-2</v>
+        <f>Input_ACEA!S9</f>
+        <v>0</v>
       </c>
       <c r="D6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="40">
-        <f>Input_ACEA!S10</f>
-        <v>3.0606000000000001E-2</v>
+        <f>Input_ACEA!S9</f>
+        <v>0</v>
       </c>
       <c r="F6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="40">
-        <f>Input_ACEA!S10</f>
-        <v>3.0606000000000001E-2</v>
+        <f>Input_ACEA!S9</f>
+        <v>0</v>
       </c>
       <c r="H6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="40">
-        <f>Input_ACEA!S10</f>
-        <v>3.0606000000000001E-2</v>
+        <f>Input_ACEA!S9</f>
+        <v>0</v>
       </c>
       <c r="J6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" s="40">
-        <f>Input_ACEA!S10</f>
-        <v>3.0606000000000001E-2</v>
+        <f>Input_ACEA!S9</f>
+        <v>0</v>
       </c>
       <c r="L6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6" s="40">
-        <f>Input_ACEA!T10</f>
-        <v>8.5252000000000008E-2</v>
+        <f>Input_ACEA!T9</f>
+        <v>0</v>
       </c>
       <c r="N6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O6" s="40">
-        <f>Input_ACEA!U10</f>
-        <v>6.8729000000000012E-2</v>
+        <f>Input_ACEA!U9</f>
+        <v>0</v>
       </c>
       <c r="P6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="40">
-        <f>Input_ACEA!S10</f>
-        <v>3.0606000000000001E-2</v>
+        <f>Input_ACEA!S9</f>
+        <v>0</v>
       </c>
       <c r="R6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S6" s="40">
-        <f>Input_ACEA!S10</f>
-        <v>3.0606000000000001E-2</v>
+        <f>Input_ACEA!S9</f>
+        <v>0</v>
       </c>
       <c r="T6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U6" s="40">
-        <f>Input_ACEA!U10</f>
-        <v>6.8729000000000012E-2</v>
+        <f>Input_ACEA!U9</f>
+        <v>0</v>
       </c>
       <c r="V6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W6" s="40">
-        <f>Input_ACEA!S10</f>
-        <v>3.0606000000000001E-2</v>
+        <f>Input_ACEA!S9</f>
+        <v>0</v>
       </c>
       <c r="X6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y6" s="40">
-        <f>Input_ACEA!T10</f>
-        <v>8.5252000000000008E-2</v>
+        <f>Input_ACEA!T9</f>
+        <v>0</v>
       </c>
       <c r="Z6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="40">
-        <f>Input_ACEA!U10</f>
-        <v>6.8729000000000012E-2</v>
+        <f>Input_ACEA!U9</f>
+        <v>0</v>
       </c>
       <c r="AB6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC6" s="40">
-        <f>Input_ACEA!S10</f>
-        <v>3.0606000000000001E-2</v>
+        <f>Input_ACEA!S9</f>
+        <v>0</v>
       </c>
       <c r="AD6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE6" s="40">
-        <f>Input_ACEA!U10</f>
-        <v>6.8729000000000012E-2</v>
+        <f>Input_ACEA!U9</f>
+        <v>0</v>
       </c>
       <c r="AF6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG6" s="40">
-        <f>Input_ACEA!S10</f>
-        <v>3.0606000000000001E-2</v>
+        <f>Input_ACEA!S9</f>
+        <v>0</v>
       </c>
       <c r="AH6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI6" s="40">
-        <f>Input_ACEA!U10</f>
-        <v>6.8729000000000012E-2</v>
+        <f>Input_ACEA!U9</f>
+        <v>0</v>
       </c>
       <c r="AJ6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK6" s="40">
-        <f>Input_ACEA!S10</f>
-        <v>3.0606000000000001E-2</v>
+        <f>Input_ACEA!S9</f>
+        <v>0</v>
       </c>
       <c r="AL6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM6" s="40">
-        <f>Input_ACEA!S10</f>
-        <v>3.0606000000000001E-2</v>
+        <f>Input_ACEA!S9</f>
+        <v>0</v>
       </c>
       <c r="AN6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO6" s="40">
-        <f>Input_ACEA!S10</f>
-        <v>3.0606000000000001E-2</v>
+        <f>Input_ACEA!S9</f>
+        <v>0</v>
       </c>
       <c r="AP6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ6" s="40">
-        <f>Input_ACEA!$V10</f>
-        <v>1.9206000000000001E-2</v>
+        <f>Input_ACEA!$V9</f>
+        <v>0</v>
       </c>
       <c r="AR6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS6" s="40">
-        <f>Input_ACEA!$V10</f>
-        <v>1.9206000000000001E-2</v>
+        <f>Input_ACEA!$V9</f>
+        <v>0</v>
       </c>
       <c r="AT6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU6" s="40">
-        <f>Input_ACEA!$V10</f>
-        <v>1.9206000000000001E-2</v>
+        <f>Input_ACEA!$V9</f>
+        <v>0</v>
       </c>
       <c r="AV6" s="24"/>
       <c r="AW6" s="24"/>
@@ -2960,165 +2860,165 @@
         <v>5</v>
       </c>
       <c r="B7" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="40">
-        <f>Input_ACEA!S11</f>
-        <v>9.2708000000000013E-2</v>
+        <f>Input_ACEA!S10</f>
+        <v>3.0606000000000001E-2</v>
       </c>
       <c r="D7" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" s="40">
-        <f>Input_ACEA!S11</f>
-        <v>9.2708000000000013E-2</v>
+        <f>Input_ACEA!S10</f>
+        <v>3.0606000000000001E-2</v>
       </c>
       <c r="F7" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" s="40">
-        <f>Input_ACEA!S11</f>
-        <v>9.2708000000000013E-2</v>
+        <f>Input_ACEA!S10</f>
+        <v>3.0606000000000001E-2</v>
       </c>
       <c r="H7" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="40">
-        <f>Input_ACEA!S11</f>
-        <v>9.2708000000000013E-2</v>
+        <f>Input_ACEA!S10</f>
+        <v>3.0606000000000001E-2</v>
       </c>
       <c r="J7" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K7" s="40">
-        <f>Input_ACEA!S11</f>
-        <v>9.2708000000000013E-2</v>
+        <f>Input_ACEA!S10</f>
+        <v>3.0606000000000001E-2</v>
       </c>
       <c r="L7" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M7" s="40">
-        <f>Input_ACEA!T11</f>
-        <v>0.29016600000000004</v>
+        <f>Input_ACEA!T10</f>
+        <v>8.5252000000000008E-2</v>
       </c>
       <c r="N7" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O7" s="40">
-        <f>Input_ACEA!U11</f>
-        <v>0.206312</v>
+        <f>Input_ACEA!U10</f>
+        <v>6.8729000000000012E-2</v>
       </c>
       <c r="P7" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q7" s="40">
-        <f>Input_ACEA!S11</f>
-        <v>9.2708000000000013E-2</v>
+        <f>Input_ACEA!S10</f>
+        <v>3.0606000000000001E-2</v>
       </c>
       <c r="R7" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S7" s="40">
-        <f>Input_ACEA!S11</f>
-        <v>9.2708000000000013E-2</v>
+        <f>Input_ACEA!S10</f>
+        <v>3.0606000000000001E-2</v>
       </c>
       <c r="T7" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U7" s="40">
-        <f>Input_ACEA!U11</f>
-        <v>0.206312</v>
+        <f>Input_ACEA!U10</f>
+        <v>6.8729000000000012E-2</v>
       </c>
       <c r="V7" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W7" s="40">
-        <f>Input_ACEA!S11</f>
-        <v>9.2708000000000013E-2</v>
+        <f>Input_ACEA!S10</f>
+        <v>3.0606000000000001E-2</v>
       </c>
       <c r="X7" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y7" s="40">
-        <f>Input_ACEA!T11</f>
-        <v>0.29016600000000004</v>
+        <f>Input_ACEA!T10</f>
+        <v>8.5252000000000008E-2</v>
       </c>
       <c r="Z7" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA7" s="40">
-        <f>Input_ACEA!U11</f>
-        <v>0.206312</v>
+        <f>Input_ACEA!U10</f>
+        <v>6.8729000000000012E-2</v>
       </c>
       <c r="AB7" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC7" s="40">
-        <f>Input_ACEA!S11</f>
-        <v>9.2708000000000013E-2</v>
+        <f>Input_ACEA!S10</f>
+        <v>3.0606000000000001E-2</v>
       </c>
       <c r="AD7" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE7" s="40">
-        <f>Input_ACEA!U11</f>
-        <v>0.206312</v>
+        <f>Input_ACEA!U10</f>
+        <v>6.8729000000000012E-2</v>
       </c>
       <c r="AF7" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG7" s="40">
-        <f>Input_ACEA!S11</f>
-        <v>9.2708000000000013E-2</v>
+        <f>Input_ACEA!S10</f>
+        <v>3.0606000000000001E-2</v>
       </c>
       <c r="AH7" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI7" s="40">
-        <f>Input_ACEA!U11</f>
-        <v>0.206312</v>
+        <f>Input_ACEA!U10</f>
+        <v>6.8729000000000012E-2</v>
       </c>
       <c r="AJ7" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK7" s="40">
-        <f>Input_ACEA!S11</f>
-        <v>9.2708000000000013E-2</v>
+        <f>Input_ACEA!S10</f>
+        <v>3.0606000000000001E-2</v>
       </c>
       <c r="AL7" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AM7" s="40">
-        <f>Input_ACEA!S11</f>
-        <v>9.2708000000000013E-2</v>
+        <f>Input_ACEA!S10</f>
+        <v>3.0606000000000001E-2</v>
       </c>
       <c r="AN7" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AO7" s="40">
-        <f>Input_ACEA!S11</f>
-        <v>9.2708000000000013E-2</v>
+        <f>Input_ACEA!S10</f>
+        <v>3.0606000000000001E-2</v>
       </c>
       <c r="AP7" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ7" s="40">
-        <f>Input_ACEA!$V11</f>
-        <v>7.4051999999999993E-2</v>
+        <f>Input_ACEA!$V10</f>
+        <v>1.9206000000000001E-2</v>
       </c>
       <c r="AR7" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AS7" s="40">
-        <f>Input_ACEA!$V11</f>
-        <v>7.4051999999999993E-2</v>
+        <f>Input_ACEA!$V10</f>
+        <v>1.9206000000000001E-2</v>
       </c>
       <c r="AT7" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AU7" s="40">
-        <f>Input_ACEA!$V11</f>
-        <v>7.4051999999999993E-2</v>
+        <f>Input_ACEA!$V10</f>
+        <v>1.9206000000000001E-2</v>
       </c>
       <c r="AV7" s="24"/>
       <c r="AW7" s="24"/>
@@ -3132,165 +3032,165 @@
         <v>5</v>
       </c>
       <c r="B8" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="40">
-        <f>Input_ACEA!S12</f>
-        <v>0.18231000000000003</v>
+        <f>Input_ACEA!S11</f>
+        <v>9.2708000000000013E-2</v>
       </c>
       <c r="D8" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" s="40">
-        <f>Input_ACEA!S12</f>
-        <v>0.18231000000000003</v>
+        <f>Input_ACEA!S11</f>
+        <v>9.2708000000000013E-2</v>
       </c>
       <c r="F8" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G8" s="40">
-        <f>Input_ACEA!S12</f>
-        <v>0.18231000000000003</v>
+        <f>Input_ACEA!S11</f>
+        <v>9.2708000000000013E-2</v>
       </c>
       <c r="H8" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I8" s="40">
-        <f>Input_ACEA!S12</f>
-        <v>0.18231000000000003</v>
+        <f>Input_ACEA!S11</f>
+        <v>9.2708000000000013E-2</v>
       </c>
       <c r="J8" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K8" s="40">
-        <f>Input_ACEA!S12</f>
-        <v>0.18231000000000003</v>
+        <f>Input_ACEA!S11</f>
+        <v>9.2708000000000013E-2</v>
       </c>
       <c r="L8" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M8" s="40">
-        <f>Input_ACEA!T12</f>
-        <v>0.5898540000000001</v>
+        <f>Input_ACEA!T11</f>
+        <v>0.29016600000000004</v>
       </c>
       <c r="N8" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O8" s="40">
-        <f>Input_ACEA!U12</f>
-        <v>0.39996900000000002</v>
+        <f>Input_ACEA!U11</f>
+        <v>0.206312</v>
       </c>
       <c r="P8" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q8" s="40">
-        <f>Input_ACEA!S12</f>
-        <v>0.18231000000000003</v>
+        <f>Input_ACEA!S11</f>
+        <v>9.2708000000000013E-2</v>
       </c>
       <c r="R8" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S8" s="40">
-        <f>Input_ACEA!S12</f>
-        <v>0.18231000000000003</v>
+        <f>Input_ACEA!S11</f>
+        <v>9.2708000000000013E-2</v>
       </c>
       <c r="T8" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U8" s="40">
-        <f>Input_ACEA!U12</f>
-        <v>0.39996900000000002</v>
+        <f>Input_ACEA!U11</f>
+        <v>0.206312</v>
       </c>
       <c r="V8" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W8" s="40">
-        <f>Input_ACEA!S12</f>
-        <v>0.18231000000000003</v>
+        <f>Input_ACEA!S11</f>
+        <v>9.2708000000000013E-2</v>
       </c>
       <c r="X8" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Y8" s="40">
-        <f>Input_ACEA!T12</f>
-        <v>0.5898540000000001</v>
+        <f>Input_ACEA!T11</f>
+        <v>0.29016600000000004</v>
       </c>
       <c r="Z8" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA8" s="40">
-        <f>Input_ACEA!U12</f>
-        <v>0.39996900000000002</v>
+        <f>Input_ACEA!U11</f>
+        <v>0.206312</v>
       </c>
       <c r="AB8" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AC8" s="40">
-        <f>Input_ACEA!S12</f>
-        <v>0.18231000000000003</v>
+        <f>Input_ACEA!S11</f>
+        <v>9.2708000000000013E-2</v>
       </c>
       <c r="AD8" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE8" s="40">
-        <f>Input_ACEA!U12</f>
-        <v>0.39996900000000002</v>
+        <f>Input_ACEA!U11</f>
+        <v>0.206312</v>
       </c>
       <c r="AF8" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG8" s="40">
-        <f>Input_ACEA!S12</f>
-        <v>0.18231000000000003</v>
+        <f>Input_ACEA!S11</f>
+        <v>9.2708000000000013E-2</v>
       </c>
       <c r="AH8" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AI8" s="40">
-        <f>Input_ACEA!U12</f>
-        <v>0.39996900000000002</v>
+        <f>Input_ACEA!U11</f>
+        <v>0.206312</v>
       </c>
       <c r="AJ8" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AK8" s="40">
-        <f>Input_ACEA!S12</f>
-        <v>0.18231000000000003</v>
+        <f>Input_ACEA!S11</f>
+        <v>9.2708000000000013E-2</v>
       </c>
       <c r="AL8" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AM8" s="40">
-        <f>Input_ACEA!S12</f>
-        <v>0.18231000000000003</v>
+        <f>Input_ACEA!S11</f>
+        <v>9.2708000000000013E-2</v>
       </c>
       <c r="AN8" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AO8" s="40">
-        <f>Input_ACEA!S12</f>
-        <v>0.18231000000000003</v>
+        <f>Input_ACEA!S11</f>
+        <v>9.2708000000000013E-2</v>
       </c>
       <c r="AP8" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AQ8" s="40">
-        <f>Input_ACEA!$V12</f>
-        <v>0.15799800000000003</v>
+        <f>Input_ACEA!$V11</f>
+        <v>7.4051999999999993E-2</v>
       </c>
       <c r="AR8" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AS8" s="40">
-        <f>Input_ACEA!$V12</f>
-        <v>0.15799800000000003</v>
+        <f>Input_ACEA!$V11</f>
+        <v>7.4051999999999993E-2</v>
       </c>
       <c r="AT8" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AU8" s="40">
-        <f>Input_ACEA!$V12</f>
-        <v>0.15799800000000003</v>
+        <f>Input_ACEA!$V11</f>
+        <v>7.4051999999999993E-2</v>
       </c>
       <c r="AV8" s="24"/>
       <c r="AW8" s="24"/>
@@ -3304,165 +3204,165 @@
         <v>5</v>
       </c>
       <c r="B9" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" s="40">
-        <f>Input_ACEA!S13</f>
-        <v>0.29541600000000001</v>
+        <f>Input_ACEA!S12</f>
+        <v>0.18231000000000003</v>
       </c>
       <c r="D9" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E9" s="40">
-        <f>Input_ACEA!S13</f>
-        <v>0.29541600000000001</v>
+        <f>Input_ACEA!S12</f>
+        <v>0.18231000000000003</v>
       </c>
       <c r="F9" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9" s="40">
-        <f>Input_ACEA!S13</f>
-        <v>0.29541600000000001</v>
+        <f>Input_ACEA!S12</f>
+        <v>0.18231000000000003</v>
       </c>
       <c r="H9" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I9" s="40">
-        <f>Input_ACEA!S13</f>
-        <v>0.29541600000000001</v>
+        <f>Input_ACEA!S12</f>
+        <v>0.18231000000000003</v>
       </c>
       <c r="J9" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K9" s="40">
-        <f>Input_ACEA!S13</f>
-        <v>0.29541600000000001</v>
+        <f>Input_ACEA!S12</f>
+        <v>0.18231000000000003</v>
       </c>
       <c r="L9" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M9" s="40">
-        <f>Input_ACEA!T13</f>
-        <v>0.95942800000000017</v>
+        <f>Input_ACEA!T12</f>
+        <v>0.5898540000000001</v>
       </c>
       <c r="N9" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O9" s="40">
-        <f>Input_ACEA!U13</f>
-        <v>0.63691999999999993</v>
+        <f>Input_ACEA!U12</f>
+        <v>0.39996900000000002</v>
       </c>
       <c r="P9" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q9" s="40">
-        <f>Input_ACEA!S13</f>
-        <v>0.29541600000000001</v>
+        <f>Input_ACEA!S12</f>
+        <v>0.18231000000000003</v>
       </c>
       <c r="R9" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S9" s="40">
-        <f>Input_ACEA!S13</f>
-        <v>0.29541600000000001</v>
+        <f>Input_ACEA!S12</f>
+        <v>0.18231000000000003</v>
       </c>
       <c r="T9" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U9" s="40">
-        <f>Input_ACEA!U13</f>
-        <v>0.63691999999999993</v>
+        <f>Input_ACEA!U12</f>
+        <v>0.39996900000000002</v>
       </c>
       <c r="V9" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W9" s="40">
-        <f>Input_ACEA!S13</f>
-        <v>0.29541600000000001</v>
+        <f>Input_ACEA!S12</f>
+        <v>0.18231000000000003</v>
       </c>
       <c r="X9" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y9" s="40">
-        <f>Input_ACEA!T13</f>
-        <v>0.95942800000000017</v>
+        <f>Input_ACEA!T12</f>
+        <v>0.5898540000000001</v>
       </c>
       <c r="Z9" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA9" s="40">
-        <f>Input_ACEA!U13</f>
-        <v>0.63691999999999993</v>
+        <f>Input_ACEA!U12</f>
+        <v>0.39996900000000002</v>
       </c>
       <c r="AB9" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC9" s="40">
-        <f>Input_ACEA!S13</f>
-        <v>0.29541600000000001</v>
+        <f>Input_ACEA!S12</f>
+        <v>0.18231000000000003</v>
       </c>
       <c r="AD9" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE9" s="40">
-        <f>Input_ACEA!U13</f>
-        <v>0.63691999999999993</v>
+        <f>Input_ACEA!U12</f>
+        <v>0.39996900000000002</v>
       </c>
       <c r="AF9" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG9" s="40">
-        <f>Input_ACEA!S13</f>
-        <v>0.29541600000000001</v>
+        <f>Input_ACEA!S12</f>
+        <v>0.18231000000000003</v>
       </c>
       <c r="AH9" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AI9" s="40">
-        <f>Input_ACEA!U13</f>
-        <v>0.63691999999999993</v>
+        <f>Input_ACEA!U12</f>
+        <v>0.39996900000000002</v>
       </c>
       <c r="AJ9" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AK9" s="40">
-        <f>Input_ACEA!S13</f>
-        <v>0.29541600000000001</v>
+        <f>Input_ACEA!S12</f>
+        <v>0.18231000000000003</v>
       </c>
       <c r="AL9" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AM9" s="40">
-        <f>Input_ACEA!S13</f>
-        <v>0.29541600000000001</v>
+        <f>Input_ACEA!S12</f>
+        <v>0.18231000000000003</v>
       </c>
       <c r="AN9" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AO9" s="40">
-        <f>Input_ACEA!S13</f>
-        <v>0.29541600000000001</v>
+        <f>Input_ACEA!S12</f>
+        <v>0.18231000000000003</v>
       </c>
       <c r="AP9" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AQ9" s="40">
-        <f>Input_ACEA!$V13</f>
-        <v>0.26450400000000002</v>
+        <f>Input_ACEA!$V12</f>
+        <v>0.15799800000000003</v>
       </c>
       <c r="AR9" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AS9" s="40">
-        <f>Input_ACEA!$V13</f>
-        <v>0.26450400000000002</v>
+        <f>Input_ACEA!$V12</f>
+        <v>0.15799800000000003</v>
       </c>
       <c r="AT9" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AU9" s="40">
-        <f>Input_ACEA!$V13</f>
-        <v>0.26450400000000002</v>
+        <f>Input_ACEA!$V12</f>
+        <v>0.15799800000000003</v>
       </c>
       <c r="AV9" s="24"/>
       <c r="AW9" s="24"/>
@@ -3476,165 +3376,165 @@
         <v>5</v>
       </c>
       <c r="B10" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="40">
-        <f>Input_ACEA!S14</f>
-        <v>0.42802999999999997</v>
+        <f>Input_ACEA!S13</f>
+        <v>0.29541600000000001</v>
       </c>
       <c r="D10" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10" s="40">
-        <f>Input_ACEA!S14</f>
-        <v>0.42802999999999997</v>
+        <f>Input_ACEA!S13</f>
+        <v>0.29541600000000001</v>
       </c>
       <c r="F10" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G10" s="40">
-        <f>Input_ACEA!S14</f>
-        <v>0.42802999999999997</v>
+        <f>Input_ACEA!S13</f>
+        <v>0.29541600000000001</v>
       </c>
       <c r="H10" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I10" s="40">
-        <f>Input_ACEA!S14</f>
-        <v>0.42802999999999997</v>
+        <f>Input_ACEA!S13</f>
+        <v>0.29541600000000001</v>
       </c>
       <c r="J10" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K10" s="40">
-        <f>Input_ACEA!S14</f>
-        <v>0.42802999999999997</v>
+        <f>Input_ACEA!S13</f>
+        <v>0.29541600000000001</v>
       </c>
       <c r="L10" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M10" s="40">
-        <f>Input_ACEA!T14</f>
-        <v>1.3740000000000001</v>
+        <f>Input_ACEA!T13</f>
+        <v>0.95942800000000017</v>
       </c>
       <c r="N10" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O10" s="40">
-        <f>Input_ACEA!U14</f>
-        <v>0.90438499999999988</v>
+        <f>Input_ACEA!U13</f>
+        <v>0.63691999999999993</v>
       </c>
       <c r="P10" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q10" s="40">
-        <f>Input_ACEA!S14</f>
-        <v>0.42802999999999997</v>
+        <f>Input_ACEA!S13</f>
+        <v>0.29541600000000001</v>
       </c>
       <c r="R10" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S10" s="40">
-        <f>Input_ACEA!S14</f>
-        <v>0.42802999999999997</v>
+        <f>Input_ACEA!S13</f>
+        <v>0.29541600000000001</v>
       </c>
       <c r="T10" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U10" s="40">
-        <f>Input_ACEA!U14</f>
-        <v>0.90438499999999988</v>
+        <f>Input_ACEA!U13</f>
+        <v>0.63691999999999993</v>
       </c>
       <c r="V10" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W10" s="40">
-        <f>Input_ACEA!S14</f>
-        <v>0.42802999999999997</v>
+        <f>Input_ACEA!S13</f>
+        <v>0.29541600000000001</v>
       </c>
       <c r="X10" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Y10" s="40">
-        <f>Input_ACEA!T14</f>
-        <v>1.3740000000000001</v>
+        <f>Input_ACEA!T13</f>
+        <v>0.95942800000000017</v>
       </c>
       <c r="Z10" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AA10" s="40">
-        <f>Input_ACEA!U14</f>
-        <v>0.90438499999999988</v>
+        <f>Input_ACEA!U13</f>
+        <v>0.63691999999999993</v>
       </c>
       <c r="AB10" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AC10" s="40">
-        <f>Input_ACEA!S14</f>
-        <v>0.42802999999999997</v>
+        <f>Input_ACEA!S13</f>
+        <v>0.29541600000000001</v>
       </c>
       <c r="AD10" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AE10" s="40">
-        <f>Input_ACEA!U14</f>
-        <v>0.90438499999999988</v>
+        <f>Input_ACEA!U13</f>
+        <v>0.63691999999999993</v>
       </c>
       <c r="AF10" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AG10" s="40">
-        <f>Input_ACEA!S14</f>
-        <v>0.42802999999999997</v>
+        <f>Input_ACEA!S13</f>
+        <v>0.29541600000000001</v>
       </c>
       <c r="AH10" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AI10" s="40">
-        <f>Input_ACEA!U14</f>
-        <v>0.90438499999999988</v>
+        <f>Input_ACEA!U13</f>
+        <v>0.63691999999999993</v>
       </c>
       <c r="AJ10" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AK10" s="40">
-        <f>Input_ACEA!S14</f>
-        <v>0.42802999999999997</v>
+        <f>Input_ACEA!S13</f>
+        <v>0.29541600000000001</v>
       </c>
       <c r="AL10" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AM10" s="40">
-        <f>Input_ACEA!S14</f>
-        <v>0.42802999999999997</v>
+        <f>Input_ACEA!S13</f>
+        <v>0.29541600000000001</v>
       </c>
       <c r="AN10" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AO10" s="40">
-        <f>Input_ACEA!S14</f>
-        <v>0.42802999999999997</v>
+        <f>Input_ACEA!S13</f>
+        <v>0.29541600000000001</v>
       </c>
       <c r="AP10" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AQ10" s="40">
-        <f>Input_ACEA!$V14</f>
-        <v>0.38702999999999999</v>
+        <f>Input_ACEA!$V13</f>
+        <v>0.26450400000000002</v>
       </c>
       <c r="AR10" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AS10" s="40">
-        <f>Input_ACEA!$V14</f>
-        <v>0.38702999999999999</v>
+        <f>Input_ACEA!$V13</f>
+        <v>0.26450400000000002</v>
       </c>
       <c r="AT10" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AU10" s="40">
-        <f>Input_ACEA!$V14</f>
-        <v>0.38702999999999999</v>
+        <f>Input_ACEA!$V13</f>
+        <v>0.26450400000000002</v>
       </c>
       <c r="AV10" s="24"/>
       <c r="AW10" s="24"/>
@@ -3648,165 +3548,165 @@
         <v>5</v>
       </c>
       <c r="B11" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="40">
-        <f>Input_ACEA!S15</f>
-        <v>0.57615600000000011</v>
+        <f>Input_ACEA!S14</f>
+        <v>0.42802999999999997</v>
       </c>
       <c r="D11" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11" s="40">
-        <f>Input_ACEA!S15</f>
-        <v>0.57615600000000011</v>
+        <f>Input_ACEA!S14</f>
+        <v>0.42802999999999997</v>
       </c>
       <c r="F11" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G11" s="40">
-        <f>Input_ACEA!S15</f>
-        <v>0.57615600000000011</v>
+        <f>Input_ACEA!S14</f>
+        <v>0.42802999999999997</v>
       </c>
       <c r="H11" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I11" s="40">
-        <f>Input_ACEA!S15</f>
-        <v>0.57615600000000011</v>
+        <f>Input_ACEA!S14</f>
+        <v>0.42802999999999997</v>
       </c>
       <c r="J11" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K11" s="40">
-        <f>Input_ACEA!S15</f>
-        <v>0.57615600000000011</v>
+        <f>Input_ACEA!S14</f>
+        <v>0.42802999999999997</v>
       </c>
       <c r="L11" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M11" s="40">
-        <f>Input_ACEA!T15</f>
-        <v>1.8086819999999999</v>
+        <f>Input_ACEA!T14</f>
+        <v>1.3740000000000001</v>
       </c>
       <c r="N11" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O11" s="40">
-        <f>Input_ACEA!U15</f>
-        <v>1.1895840000000002</v>
+        <f>Input_ACEA!U14</f>
+        <v>0.90438499999999988</v>
       </c>
       <c r="P11" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q11" s="40">
-        <f>Input_ACEA!S15</f>
-        <v>0.57615600000000011</v>
+        <f>Input_ACEA!S14</f>
+        <v>0.42802999999999997</v>
       </c>
       <c r="R11" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S11" s="40">
-        <f>Input_ACEA!S15</f>
-        <v>0.57615600000000011</v>
+        <f>Input_ACEA!S14</f>
+        <v>0.42802999999999997</v>
       </c>
       <c r="T11" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U11" s="40">
-        <f>Input_ACEA!U15</f>
-        <v>1.1895840000000002</v>
+        <f>Input_ACEA!U14</f>
+        <v>0.90438499999999988</v>
       </c>
       <c r="V11" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W11" s="40">
-        <f>Input_ACEA!S15</f>
-        <v>0.57615600000000011</v>
+        <f>Input_ACEA!S14</f>
+        <v>0.42802999999999997</v>
       </c>
       <c r="X11" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Y11" s="40">
-        <f>Input_ACEA!T15</f>
-        <v>1.8086819999999999</v>
+        <f>Input_ACEA!T14</f>
+        <v>1.3740000000000001</v>
       </c>
       <c r="Z11" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AA11" s="40">
-        <f>Input_ACEA!U15</f>
-        <v>1.1895840000000002</v>
+        <f>Input_ACEA!U14</f>
+        <v>0.90438499999999988</v>
       </c>
       <c r="AB11" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AC11" s="40">
-        <f>Input_ACEA!S15</f>
-        <v>0.57615600000000011</v>
+        <f>Input_ACEA!S14</f>
+        <v>0.42802999999999997</v>
       </c>
       <c r="AD11" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AE11" s="40">
-        <f>Input_ACEA!U15</f>
-        <v>1.1895840000000002</v>
+        <f>Input_ACEA!U14</f>
+        <v>0.90438499999999988</v>
       </c>
       <c r="AF11" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AG11" s="40">
-        <f>Input_ACEA!S15</f>
-        <v>0.57615600000000011</v>
+        <f>Input_ACEA!S14</f>
+        <v>0.42802999999999997</v>
       </c>
       <c r="AH11" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AI11" s="40">
-        <f>Input_ACEA!U15</f>
-        <v>1.1895840000000002</v>
+        <f>Input_ACEA!U14</f>
+        <v>0.90438499999999988</v>
       </c>
       <c r="AJ11" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AK11" s="40">
-        <f>Input_ACEA!S15</f>
-        <v>0.57615600000000011</v>
+        <f>Input_ACEA!S14</f>
+        <v>0.42802999999999997</v>
       </c>
       <c r="AL11" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AM11" s="40">
-        <f>Input_ACEA!S15</f>
-        <v>0.57615600000000011</v>
+        <f>Input_ACEA!S14</f>
+        <v>0.42802999999999997</v>
       </c>
       <c r="AN11" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AO11" s="40">
-        <f>Input_ACEA!S15</f>
-        <v>0.57615600000000011</v>
+        <f>Input_ACEA!S14</f>
+        <v>0.42802999999999997</v>
       </c>
       <c r="AP11" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AQ11" s="40">
-        <f>Input_ACEA!$V15</f>
-        <v>0.51903600000000005</v>
+        <f>Input_ACEA!$V14</f>
+        <v>0.38702999999999999</v>
       </c>
       <c r="AR11" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AS11" s="40">
-        <f>Input_ACEA!$V15</f>
-        <v>0.51903600000000005</v>
+        <f>Input_ACEA!$V14</f>
+        <v>0.38702999999999999</v>
       </c>
       <c r="AT11" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AU11" s="40">
-        <f>Input_ACEA!$V15</f>
-        <v>0.51903600000000005</v>
+        <f>Input_ACEA!$V14</f>
+        <v>0.38702999999999999</v>
       </c>
       <c r="AV11" s="24"/>
       <c r="AW11" s="24"/>
@@ -3816,169 +3716,169 @@
       <c r="BA11" s="24"/>
     </row>
     <row r="12" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="40">
-        <f>Input_ACEA!S16</f>
-        <v>0.73579800000000006</v>
+        <f>Input_ACEA!S15</f>
+        <v>0.57615600000000011</v>
       </c>
       <c r="D12" s="39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12" s="40">
-        <f>Input_ACEA!S16</f>
-        <v>0.73579800000000006</v>
+        <f>Input_ACEA!S15</f>
+        <v>0.57615600000000011</v>
       </c>
       <c r="F12" s="39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G12" s="40">
-        <f>Input_ACEA!S16</f>
-        <v>0.73579800000000006</v>
+        <f>Input_ACEA!S15</f>
+        <v>0.57615600000000011</v>
       </c>
       <c r="H12" s="39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I12" s="40">
-        <f>Input_ACEA!S16</f>
-        <v>0.73579800000000006</v>
+        <f>Input_ACEA!S15</f>
+        <v>0.57615600000000011</v>
       </c>
       <c r="J12" s="39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K12" s="40">
-        <f>Input_ACEA!S16</f>
-        <v>0.73579800000000006</v>
+        <f>Input_ACEA!S15</f>
+        <v>0.57615600000000011</v>
       </c>
       <c r="L12" s="39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M12" s="40">
-        <f>Input_ACEA!T16</f>
-        <v>2.2385860000000006</v>
+        <f>Input_ACEA!T15</f>
+        <v>1.8086819999999999</v>
       </c>
       <c r="N12" s="39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O12" s="40">
-        <f>Input_ACEA!U16</f>
-        <v>1.4797370000000005</v>
+        <f>Input_ACEA!U15</f>
+        <v>1.1895840000000002</v>
       </c>
       <c r="P12" s="39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q12" s="40">
-        <f>Input_ACEA!S16</f>
-        <v>0.73579800000000006</v>
+        <f>Input_ACEA!S15</f>
+        <v>0.57615600000000011</v>
       </c>
       <c r="R12" s="39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S12" s="40">
-        <f>Input_ACEA!S16</f>
-        <v>0.73579800000000006</v>
+        <f>Input_ACEA!S15</f>
+        <v>0.57615600000000011</v>
       </c>
       <c r="T12" s="39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U12" s="40">
-        <f>Input_ACEA!U16</f>
-        <v>1.4797370000000005</v>
+        <f>Input_ACEA!U15</f>
+        <v>1.1895840000000002</v>
       </c>
       <c r="V12" s="39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W12" s="40">
-        <f>Input_ACEA!S16</f>
-        <v>0.73579800000000006</v>
+        <f>Input_ACEA!S15</f>
+        <v>0.57615600000000011</v>
       </c>
       <c r="X12" s="39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Y12" s="40">
-        <f>Input_ACEA!T16</f>
-        <v>2.2385860000000006</v>
+        <f>Input_ACEA!T15</f>
+        <v>1.8086819999999999</v>
       </c>
       <c r="Z12" s="39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA12" s="40">
-        <f>Input_ACEA!U16</f>
-        <v>1.4797370000000005</v>
+        <f>Input_ACEA!U15</f>
+        <v>1.1895840000000002</v>
       </c>
       <c r="AB12" s="39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AC12" s="40">
-        <f>Input_ACEA!S16</f>
-        <v>0.73579800000000006</v>
+        <f>Input_ACEA!S15</f>
+        <v>0.57615600000000011</v>
       </c>
       <c r="AD12" s="39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AE12" s="40">
-        <f>Input_ACEA!U16</f>
-        <v>1.4797370000000005</v>
+        <f>Input_ACEA!U15</f>
+        <v>1.1895840000000002</v>
       </c>
       <c r="AF12" s="39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AG12" s="40">
-        <f>Input_ACEA!S16</f>
-        <v>0.73579800000000006</v>
+        <f>Input_ACEA!S15</f>
+        <v>0.57615600000000011</v>
       </c>
       <c r="AH12" s="39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AI12" s="40">
-        <f>Input_ACEA!U16</f>
-        <v>1.4797370000000005</v>
+        <f>Input_ACEA!U15</f>
+        <v>1.1895840000000002</v>
       </c>
       <c r="AJ12" s="39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AK12" s="40">
-        <f>Input_ACEA!S16</f>
-        <v>0.73579800000000006</v>
+        <f>Input_ACEA!S15</f>
+        <v>0.57615600000000011</v>
       </c>
       <c r="AL12" s="39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AM12" s="40">
-        <f>Input_ACEA!S16</f>
-        <v>0.73579800000000006</v>
+        <f>Input_ACEA!S15</f>
+        <v>0.57615600000000011</v>
       </c>
       <c r="AN12" s="39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AO12" s="40">
-        <f>Input_ACEA!S16</f>
-        <v>0.73579800000000006</v>
+        <f>Input_ACEA!S15</f>
+        <v>0.57615600000000011</v>
       </c>
       <c r="AP12" s="39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AQ12" s="40">
-        <f>Input_ACEA!$V16</f>
-        <v>0.65398200000000017</v>
+        <f>Input_ACEA!$V15</f>
+        <v>0.51903600000000005</v>
       </c>
       <c r="AR12" s="39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AS12" s="40">
-        <f>Input_ACEA!$V16</f>
-        <v>0.65398200000000017</v>
+        <f>Input_ACEA!$V15</f>
+        <v>0.51903600000000005</v>
       </c>
       <c r="AT12" s="39">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AU12" s="40">
-        <f>Input_ACEA!$V16</f>
-        <v>0.65398200000000017</v>
+        <f>Input_ACEA!$V15</f>
+        <v>0.51903600000000005</v>
       </c>
       <c r="AV12" s="24"/>
       <c r="AW12" s="24"/>
@@ -3992,165 +3892,165 @@
         <v>5</v>
       </c>
       <c r="B13" s="39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="40">
-        <f>Input_ACEA!S17</f>
-        <v>0.90296000000000021</v>
+        <f>Input_ACEA!S16</f>
+        <v>0.73579800000000006</v>
       </c>
       <c r="D13" s="39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" s="40">
-        <f>Input_ACEA!S17</f>
-        <v>0.90296000000000021</v>
+        <f>Input_ACEA!S16</f>
+        <v>0.73579800000000006</v>
       </c>
       <c r="F13" s="39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G13" s="40">
-        <f>Input_ACEA!S17</f>
-        <v>0.90296000000000021</v>
+        <f>Input_ACEA!S16</f>
+        <v>0.73579800000000006</v>
       </c>
       <c r="H13" s="39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I13" s="40">
-        <f>Input_ACEA!S17</f>
-        <v>0.90296000000000021</v>
+        <f>Input_ACEA!S16</f>
+        <v>0.73579800000000006</v>
       </c>
       <c r="J13" s="39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K13" s="40">
-        <f>Input_ACEA!S17</f>
-        <v>0.90296000000000021</v>
+        <f>Input_ACEA!S16</f>
+        <v>0.73579800000000006</v>
       </c>
       <c r="L13" s="39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M13" s="40">
-        <f>Input_ACEA!T17</f>
-        <v>2.6388240000000009</v>
+        <f>Input_ACEA!T16</f>
+        <v>2.2385860000000006</v>
       </c>
       <c r="N13" s="39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O13" s="40">
-        <f>Input_ACEA!U17</f>
-        <v>1.7620640000000001</v>
+        <f>Input_ACEA!U16</f>
+        <v>1.4797370000000005</v>
       </c>
       <c r="P13" s="39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q13" s="40">
-        <f>Input_ACEA!S17</f>
-        <v>0.90296000000000021</v>
+        <f>Input_ACEA!S16</f>
+        <v>0.73579800000000006</v>
       </c>
       <c r="R13" s="39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="S13" s="40">
-        <f>Input_ACEA!S17</f>
-        <v>0.90296000000000021</v>
+        <f>Input_ACEA!S16</f>
+        <v>0.73579800000000006</v>
       </c>
       <c r="T13" s="39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="U13" s="40">
-        <f>Input_ACEA!U17</f>
-        <v>1.7620640000000001</v>
+        <f>Input_ACEA!U16</f>
+        <v>1.4797370000000005</v>
       </c>
       <c r="V13" s="39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="W13" s="40">
-        <f>Input_ACEA!S17</f>
-        <v>0.90296000000000021</v>
+        <f>Input_ACEA!S16</f>
+        <v>0.73579800000000006</v>
       </c>
       <c r="X13" s="39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Y13" s="40">
-        <f>Input_ACEA!T17</f>
-        <v>2.6388240000000009</v>
+        <f>Input_ACEA!T16</f>
+        <v>2.2385860000000006</v>
       </c>
       <c r="Z13" s="39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AA13" s="40">
-        <f>Input_ACEA!U17</f>
-        <v>1.7620640000000001</v>
+        <f>Input_ACEA!U16</f>
+        <v>1.4797370000000005</v>
       </c>
       <c r="AB13" s="39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AC13" s="40">
-        <f>Input_ACEA!S17</f>
-        <v>0.90296000000000021</v>
+        <f>Input_ACEA!S16</f>
+        <v>0.73579800000000006</v>
       </c>
       <c r="AD13" s="39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AE13" s="40">
-        <f>Input_ACEA!U17</f>
-        <v>1.7620640000000001</v>
+        <f>Input_ACEA!U16</f>
+        <v>1.4797370000000005</v>
       </c>
       <c r="AF13" s="39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AG13" s="40">
-        <f>Input_ACEA!S17</f>
-        <v>0.90296000000000021</v>
+        <f>Input_ACEA!S16</f>
+        <v>0.73579800000000006</v>
       </c>
       <c r="AH13" s="39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AI13" s="40">
-        <f>Input_ACEA!U17</f>
-        <v>1.7620640000000001</v>
+        <f>Input_ACEA!U16</f>
+        <v>1.4797370000000005</v>
       </c>
       <c r="AJ13" s="39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AK13" s="40">
-        <f>Input_ACEA!S17</f>
-        <v>0.90296000000000021</v>
+        <f>Input_ACEA!S16</f>
+        <v>0.73579800000000006</v>
       </c>
       <c r="AL13" s="39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AM13" s="40">
-        <f>Input_ACEA!S17</f>
-        <v>0.90296000000000021</v>
+        <f>Input_ACEA!S16</f>
+        <v>0.73579800000000006</v>
       </c>
       <c r="AN13" s="39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AO13" s="40">
-        <f>Input_ACEA!S17</f>
-        <v>0.90296000000000021</v>
+        <f>Input_ACEA!S16</f>
+        <v>0.73579800000000006</v>
       </c>
       <c r="AP13" s="39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AQ13" s="40">
-        <f>Input_ACEA!$V17</f>
-        <v>0.78532800000000014</v>
+        <f>Input_ACEA!$V16</f>
+        <v>0.65398200000000017</v>
       </c>
       <c r="AR13" s="39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AS13" s="40">
-        <f>Input_ACEA!$V17</f>
-        <v>0.78532800000000014</v>
+        <f>Input_ACEA!$V16</f>
+        <v>0.65398200000000017</v>
       </c>
       <c r="AT13" s="39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AU13" s="40">
-        <f>Input_ACEA!$V17</f>
-        <v>0.78532800000000014</v>
+        <f>Input_ACEA!$V16</f>
+        <v>0.65398200000000017</v>
       </c>
       <c r="AV13" s="24"/>
       <c r="AW13" s="24"/>
@@ -4164,165 +4064,165 @@
         <v>5</v>
       </c>
       <c r="B14" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" s="40">
-        <f>Input_ACEA!S18</f>
-        <v>1.0736460000000003</v>
+        <f>Input_ACEA!S17</f>
+        <v>0.90296000000000021</v>
       </c>
       <c r="D14" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" s="40">
-        <f>Input_ACEA!S18</f>
-        <v>1.0736460000000003</v>
+        <f>Input_ACEA!S17</f>
+        <v>0.90296000000000021</v>
       </c>
       <c r="F14" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G14" s="40">
-        <f>Input_ACEA!S18</f>
-        <v>1.0736460000000003</v>
+        <f>Input_ACEA!S17</f>
+        <v>0.90296000000000021</v>
       </c>
       <c r="H14" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I14" s="40">
-        <f>Input_ACEA!S18</f>
-        <v>1.0736460000000003</v>
+        <f>Input_ACEA!S17</f>
+        <v>0.90296000000000021</v>
       </c>
       <c r="J14" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K14" s="40">
-        <f>Input_ACEA!S18</f>
-        <v>1.0736460000000003</v>
+        <f>Input_ACEA!S17</f>
+        <v>0.90296000000000021</v>
       </c>
       <c r="L14" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M14" s="40">
-        <f>Input_ACEA!T18</f>
-        <v>2.9845080000000004</v>
+        <f>Input_ACEA!T17</f>
+        <v>2.6388240000000009</v>
       </c>
       <c r="N14" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O14" s="40">
-        <f>Input_ACEA!U18</f>
-        <v>2.0237850000000002</v>
+        <f>Input_ACEA!U17</f>
+        <v>1.7620640000000001</v>
       </c>
       <c r="P14" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q14" s="40">
-        <f>Input_ACEA!S18</f>
-        <v>1.0736460000000003</v>
+        <f>Input_ACEA!S17</f>
+        <v>0.90296000000000021</v>
       </c>
       <c r="R14" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S14" s="40">
-        <f>Input_ACEA!S18</f>
-        <v>1.0736460000000003</v>
+        <f>Input_ACEA!S17</f>
+        <v>0.90296000000000021</v>
       </c>
       <c r="T14" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U14" s="40">
-        <f>Input_ACEA!U18</f>
-        <v>2.0237850000000002</v>
+        <f>Input_ACEA!U17</f>
+        <v>1.7620640000000001</v>
       </c>
       <c r="V14" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W14" s="40">
-        <f>Input_ACEA!S18</f>
-        <v>1.0736460000000003</v>
+        <f>Input_ACEA!S17</f>
+        <v>0.90296000000000021</v>
       </c>
       <c r="X14" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Y14" s="40">
-        <f>Input_ACEA!T18</f>
-        <v>2.9845080000000004</v>
+        <f>Input_ACEA!T17</f>
+        <v>2.6388240000000009</v>
       </c>
       <c r="Z14" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AA14" s="40">
-        <f>Input_ACEA!U18</f>
-        <v>2.0237850000000002</v>
+        <f>Input_ACEA!U17</f>
+        <v>1.7620640000000001</v>
       </c>
       <c r="AB14" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AC14" s="40">
-        <f>Input_ACEA!S18</f>
-        <v>1.0736460000000003</v>
+        <f>Input_ACEA!S17</f>
+        <v>0.90296000000000021</v>
       </c>
       <c r="AD14" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AE14" s="40">
-        <f>Input_ACEA!U18</f>
-        <v>2.0237850000000002</v>
+        <f>Input_ACEA!U17</f>
+        <v>1.7620640000000001</v>
       </c>
       <c r="AF14" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AG14" s="40">
-        <f>Input_ACEA!S18</f>
-        <v>1.0736460000000003</v>
+        <f>Input_ACEA!S17</f>
+        <v>0.90296000000000021</v>
       </c>
       <c r="AH14" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AI14" s="40">
-        <f>Input_ACEA!U18</f>
-        <v>2.0237850000000002</v>
+        <f>Input_ACEA!U17</f>
+        <v>1.7620640000000001</v>
       </c>
       <c r="AJ14" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AK14" s="40">
-        <f>Input_ACEA!S18</f>
-        <v>1.0736460000000003</v>
+        <f>Input_ACEA!S17</f>
+        <v>0.90296000000000021</v>
       </c>
       <c r="AL14" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AM14" s="40">
-        <f>Input_ACEA!S18</f>
-        <v>1.0736460000000003</v>
+        <f>Input_ACEA!S17</f>
+        <v>0.90296000000000021</v>
       </c>
       <c r="AN14" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AO14" s="40">
-        <f>Input_ACEA!S18</f>
-        <v>1.0736460000000003</v>
+        <f>Input_ACEA!S17</f>
+        <v>0.90296000000000021</v>
       </c>
       <c r="AP14" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AQ14" s="40">
-        <f>Input_ACEA!$V18</f>
-        <v>0.90653399999999995</v>
+        <f>Input_ACEA!$V17</f>
+        <v>0.78532800000000014</v>
       </c>
       <c r="AR14" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AS14" s="40">
-        <f>Input_ACEA!$V18</f>
-        <v>0.90653399999999995</v>
+        <f>Input_ACEA!$V17</f>
+        <v>0.78532800000000014</v>
       </c>
       <c r="AT14" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AU14" s="40">
-        <f>Input_ACEA!$V18</f>
-        <v>0.90653399999999995</v>
+        <f>Input_ACEA!$V17</f>
+        <v>0.78532800000000014</v>
       </c>
       <c r="AV14" s="24"/>
       <c r="AW14" s="24"/>
@@ -4336,165 +4236,165 @@
         <v>5</v>
       </c>
       <c r="B15" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="40">
-        <f>Input_ACEA!S19</f>
-        <v>1.2438599999999997</v>
+        <f>Input_ACEA!S18</f>
+        <v>1.0736460000000003</v>
       </c>
       <c r="D15" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" s="40">
-        <f>Input_ACEA!S19</f>
-        <v>1.2438599999999997</v>
+        <f>Input_ACEA!S18</f>
+        <v>1.0736460000000003</v>
       </c>
       <c r="F15" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G15" s="40">
-        <f>Input_ACEA!S19</f>
-        <v>1.2438599999999997</v>
+        <f>Input_ACEA!S18</f>
+        <v>1.0736460000000003</v>
       </c>
       <c r="H15" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I15" s="40">
-        <f>Input_ACEA!S19</f>
-        <v>1.2438599999999997</v>
+        <f>Input_ACEA!S18</f>
+        <v>1.0736460000000003</v>
       </c>
       <c r="J15" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K15" s="40">
-        <f>Input_ACEA!S19</f>
-        <v>1.2438599999999997</v>
+        <f>Input_ACEA!S18</f>
+        <v>1.0736460000000003</v>
       </c>
       <c r="L15" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M15" s="40">
-        <f>Input_ACEA!T19</f>
-        <v>3.25075</v>
+        <f>Input_ACEA!T18</f>
+        <v>2.9845080000000004</v>
       </c>
       <c r="N15" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O15" s="40">
-        <f>Input_ACEA!U19</f>
-        <v>2.2521199999999997</v>
+        <f>Input_ACEA!U18</f>
+        <v>2.0237850000000002</v>
       </c>
       <c r="P15" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q15" s="40">
-        <f>Input_ACEA!S19</f>
-        <v>1.2438599999999997</v>
+        <f>Input_ACEA!S18</f>
+        <v>1.0736460000000003</v>
       </c>
       <c r="R15" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="S15" s="40">
-        <f>Input_ACEA!S19</f>
-        <v>1.2438599999999997</v>
+        <f>Input_ACEA!S18</f>
+        <v>1.0736460000000003</v>
       </c>
       <c r="T15" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="U15" s="40">
-        <f>Input_ACEA!U19</f>
-        <v>2.2521199999999997</v>
+        <f>Input_ACEA!U18</f>
+        <v>2.0237850000000002</v>
       </c>
       <c r="V15" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="W15" s="40">
-        <f>Input_ACEA!S19</f>
-        <v>1.2438599999999997</v>
+        <f>Input_ACEA!S18</f>
+        <v>1.0736460000000003</v>
       </c>
       <c r="X15" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Y15" s="40">
-        <f>Input_ACEA!T19</f>
-        <v>3.25075</v>
+        <f>Input_ACEA!T18</f>
+        <v>2.9845080000000004</v>
       </c>
       <c r="Z15" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AA15" s="40">
-        <f>Input_ACEA!U19</f>
-        <v>2.2521199999999997</v>
+        <f>Input_ACEA!U18</f>
+        <v>2.0237850000000002</v>
       </c>
       <c r="AB15" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC15" s="40">
-        <f>Input_ACEA!S19</f>
-        <v>1.2438599999999997</v>
+        <f>Input_ACEA!S18</f>
+        <v>1.0736460000000003</v>
       </c>
       <c r="AD15" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AE15" s="40">
-        <f>Input_ACEA!U19</f>
-        <v>2.2521199999999997</v>
+        <f>Input_ACEA!U18</f>
+        <v>2.0237850000000002</v>
       </c>
       <c r="AF15" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AG15" s="40">
-        <f>Input_ACEA!S19</f>
-        <v>1.2438599999999997</v>
+        <f>Input_ACEA!S18</f>
+        <v>1.0736460000000003</v>
       </c>
       <c r="AH15" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AI15" s="40">
-        <f>Input_ACEA!U19</f>
-        <v>2.2521199999999997</v>
+        <f>Input_ACEA!U18</f>
+        <v>2.0237850000000002</v>
       </c>
       <c r="AJ15" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AK15" s="40">
-        <f>Input_ACEA!S19</f>
-        <v>1.2438599999999997</v>
+        <f>Input_ACEA!S18</f>
+        <v>1.0736460000000003</v>
       </c>
       <c r="AL15" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AM15" s="40">
-        <f>Input_ACEA!S19</f>
-        <v>1.2438599999999997</v>
+        <f>Input_ACEA!S18</f>
+        <v>1.0736460000000003</v>
       </c>
       <c r="AN15" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AO15" s="40">
-        <f>Input_ACEA!S19</f>
-        <v>1.2438599999999997</v>
+        <f>Input_ACEA!S18</f>
+        <v>1.0736460000000003</v>
       </c>
       <c r="AP15" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AQ15" s="40">
-        <f>Input_ACEA!$V19</f>
-        <v>1.0110599999999998</v>
+        <f>Input_ACEA!$V18</f>
+        <v>0.90653399999999995</v>
       </c>
       <c r="AR15" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AS15" s="40">
-        <f>Input_ACEA!$V19</f>
-        <v>1.0110599999999998</v>
+        <f>Input_ACEA!$V18</f>
+        <v>0.90653399999999995</v>
       </c>
       <c r="AT15" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AU15" s="40">
-        <f>Input_ACEA!$V19</f>
-        <v>1.0110599999999998</v>
+        <f>Input_ACEA!$V18</f>
+        <v>0.90653399999999995</v>
       </c>
       <c r="AV15" s="24"/>
       <c r="AW15" s="24"/>
@@ -4504,7 +4404,176 @@
       <c r="BA15" s="24"/>
     </row>
     <row r="16" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
+      <c r="A16" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="39">
+        <v>10</v>
+      </c>
+      <c r="C16" s="40">
+        <f>Input_ACEA!S19</f>
+        <v>1.2438599999999997</v>
+      </c>
+      <c r="D16" s="39">
+        <v>10</v>
+      </c>
+      <c r="E16" s="40">
+        <f>Input_ACEA!S19</f>
+        <v>1.2438599999999997</v>
+      </c>
+      <c r="F16" s="39">
+        <v>10</v>
+      </c>
+      <c r="G16" s="40">
+        <f>Input_ACEA!S19</f>
+        <v>1.2438599999999997</v>
+      </c>
+      <c r="H16" s="39">
+        <v>10</v>
+      </c>
+      <c r="I16" s="40">
+        <f>Input_ACEA!S19</f>
+        <v>1.2438599999999997</v>
+      </c>
+      <c r="J16" s="39">
+        <v>10</v>
+      </c>
+      <c r="K16" s="40">
+        <f>Input_ACEA!S19</f>
+        <v>1.2438599999999997</v>
+      </c>
+      <c r="L16" s="39">
+        <v>10</v>
+      </c>
+      <c r="M16" s="40">
+        <f>Input_ACEA!T19</f>
+        <v>3.25075</v>
+      </c>
+      <c r="N16" s="39">
+        <v>10</v>
+      </c>
+      <c r="O16" s="40">
+        <f>Input_ACEA!U19</f>
+        <v>2.2521199999999997</v>
+      </c>
+      <c r="P16" s="39">
+        <v>10</v>
+      </c>
+      <c r="Q16" s="40">
+        <f>Input_ACEA!S19</f>
+        <v>1.2438599999999997</v>
+      </c>
+      <c r="R16" s="39">
+        <v>10</v>
+      </c>
+      <c r="S16" s="40">
+        <f>Input_ACEA!S19</f>
+        <v>1.2438599999999997</v>
+      </c>
+      <c r="T16" s="39">
+        <v>10</v>
+      </c>
+      <c r="U16" s="40">
+        <f>Input_ACEA!U19</f>
+        <v>2.2521199999999997</v>
+      </c>
+      <c r="V16" s="39">
+        <v>10</v>
+      </c>
+      <c r="W16" s="40">
+        <f>Input_ACEA!S19</f>
+        <v>1.2438599999999997</v>
+      </c>
+      <c r="X16" s="39">
+        <v>10</v>
+      </c>
+      <c r="Y16" s="40">
+        <f>Input_ACEA!T19</f>
+        <v>3.25075</v>
+      </c>
+      <c r="Z16" s="39">
+        <v>10</v>
+      </c>
+      <c r="AA16" s="40">
+        <f>Input_ACEA!U19</f>
+        <v>2.2521199999999997</v>
+      </c>
+      <c r="AB16" s="39">
+        <v>10</v>
+      </c>
+      <c r="AC16" s="40">
+        <f>Input_ACEA!S19</f>
+        <v>1.2438599999999997</v>
+      </c>
+      <c r="AD16" s="39">
+        <v>10</v>
+      </c>
+      <c r="AE16" s="40">
+        <f>Input_ACEA!U19</f>
+        <v>2.2521199999999997</v>
+      </c>
+      <c r="AF16" s="39">
+        <v>10</v>
+      </c>
+      <c r="AG16" s="40">
+        <f>Input_ACEA!S19</f>
+        <v>1.2438599999999997</v>
+      </c>
+      <c r="AH16" s="39">
+        <v>10</v>
+      </c>
+      <c r="AI16" s="40">
+        <f>Input_ACEA!U19</f>
+        <v>2.2521199999999997</v>
+      </c>
+      <c r="AJ16" s="39">
+        <v>10</v>
+      </c>
+      <c r="AK16" s="40">
+        <f>Input_ACEA!S19</f>
+        <v>1.2438599999999997</v>
+      </c>
+      <c r="AL16" s="39">
+        <v>10</v>
+      </c>
+      <c r="AM16" s="40">
+        <f>Input_ACEA!S19</f>
+        <v>1.2438599999999997</v>
+      </c>
+      <c r="AN16" s="39">
+        <v>10</v>
+      </c>
+      <c r="AO16" s="40">
+        <f>Input_ACEA!S19</f>
+        <v>1.2438599999999997</v>
+      </c>
+      <c r="AP16" s="39">
+        <v>10</v>
+      </c>
+      <c r="AQ16" s="40">
+        <f>Input_ACEA!$V19</f>
+        <v>1.0110599999999998</v>
+      </c>
+      <c r="AR16" s="39">
+        <v>10</v>
+      </c>
+      <c r="AS16" s="40">
+        <f>Input_ACEA!$V19</f>
+        <v>1.0110599999999998</v>
+      </c>
+      <c r="AT16" s="39">
+        <v>10</v>
+      </c>
+      <c r="AU16" s="40">
+        <f>Input_ACEA!$V19</f>
+        <v>1.0110599999999998</v>
+      </c>
+      <c r="AV16" s="24"/>
+      <c r="AW16" s="24"/>
+      <c r="AX16" s="24"/>
+      <c r="AY16" s="24"/>
+      <c r="AZ16" s="24"/>
+      <c r="BA16" s="24"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
@@ -4517,6 +4586,9 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="24"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -4527,8 +4599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="R3:V33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AB19" sqref="AB19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4977,7 +5049,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="44"/>
-      <c r="B6" s="47"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
@@ -4990,7 +5062,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="44"/>
-      <c r="B7" s="47"/>
+      <c r="B7" s="50"/>
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
@@ -5003,7 +5075,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="44"/>
-      <c r="B8" s="47"/>
+      <c r="B8" s="50"/>
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
@@ -5016,7 +5088,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="44"/>
-      <c r="B9" s="48"/>
+      <c r="B9" s="47"/>
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
@@ -5029,7 +5101,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="44"/>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="48" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -5044,7 +5116,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="44"/>
-      <c r="B11" s="47"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
@@ -5057,7 +5129,7 @@
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="45"/>
-      <c r="B12" s="50"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="7" t="s">
         <v>20</v>
       </c>
@@ -5087,7 +5159,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="44"/>
-      <c r="B14" s="48"/>
+      <c r="B14" s="47"/>
       <c r="C14" s="1" t="s">
         <v>20</v>
       </c>
@@ -5100,7 +5172,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="44"/>
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="48" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -5115,7 +5187,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="44"/>
-      <c r="B16" s="48"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="1" t="s">
         <v>20</v>
       </c>
@@ -5128,7 +5200,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="44"/>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="48" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -5143,7 +5215,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="45"/>
-      <c r="B18" s="50"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="7" t="s">
         <v>20</v>
       </c>
@@ -5238,16 +5310,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A5:A12"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:E2"/>
     <mergeCell ref="A13:A18"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A5:A12"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>